<commit_message>
checking code works on Emilys laptop
</commit_message>
<xml_diff>
--- a/Split_mechanics/comparison.xlsx
+++ b/Split_mechanics/comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egrout\Dropbox\coatithon\coatithon_code\Split_mechanics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F3F479-E032-4B73-9570-9F874D23438D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414842F1-4A37-460B-8269-FD8F32DDAEFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12140" windowHeight="7070" xr2:uid="{2CC02707-5C96-4E02-B9BA-CC98DE0C03C0}"/>
   </bookViews>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD42E3F-6C50-45F6-9CF7-93419C3713DC}">
   <dimension ref="A1:O490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H222" sqref="H222"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>